<commit_message>
updated narrative tables, bbdd and dict
</commit_message>
<xml_diff>
--- a/excel_books/bbdd_sfdr_wip.xlsx
+++ b/excel_books/bbdd_sfdr_wip.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://santandernet.sharepoint.com/sites/ESGTEAM552/Shared Documents/Archivos/Archivos Red/Fondos éticos/09. REGULACIÓN/04_SFDR/Info_Periódica/Revisión_generación/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n740789\Documents\sfdr_report_generator\excel_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="755" documentId="8_{BBF384ED-78AF-47CF-9DFA-BD9893418057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50F8F86C-DDD9-4313-89AC-EF72E7DED6C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F06AA4-4A01-44BE-B2C5-EB653B38B475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15435" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{E9EDE50E-DEA4-4E38-B493-23471F5C8DA9}"/>
+    <workbookView xWindow="14760" yWindow="-16470" windowWidth="29040" windowHeight="16440" xr2:uid="{E9EDE50E-DEA4-4E38-B493-23471F5C8DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$150</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1691,7 +1691,7 @@
     <t>PFIT0516</t>
   </si>
   <si>
-    <t>Fundo De Investimento Mobiliário Aberto de Ações Santander Acções Europa</t>
+    <t>Fundo de Investimento Mobiliário Aberto de Ações Santander Acções Europa</t>
   </si>
   <si>
     <t>5493000MEK7GQ3X3RT85. ISIN: PTYSADLM0008; PTYSANHM0002</t>
@@ -1706,7 +1706,7 @@
     <t>PFIT0605</t>
   </si>
   <si>
-    <t>Fundo De Investimento Alternativo Aberto de Poupança Reforma Santander Poupança Prudente FPR</t>
+    <t>Fundo de Investimento Alternativo Aberto de Poupança Reforma Santander Poupança Prudente FPR</t>
   </si>
   <si>
     <t>5493004I3WS5T3F63O98. ISIN: PTYSAVLM0006</t>
@@ -1796,9 +1796,6 @@
     <t>PFIT1830</t>
   </si>
   <si>
-    <t>Fundo de Investimento Mobiliário Aberto de Obrigações de Poupança Reforma Santander Aforro PPR/OICVM</t>
-  </si>
-  <si>
     <t>549300NK9YXGJCPV4J35. ISIN: PTSFFAHM0013</t>
   </si>
   <si>
@@ -1911,13 +1908,16 @@
   </si>
   <si>
     <t>12/12/2024 - 31/12/2024</t>
+  </si>
+  <si>
+    <t>Fundo de Investimento Mobiliário Aberto de Obrigações de Poupança Reforma Santander Aforro PPR OICVM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1959,13 +1959,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Santander Text"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -2166,9 +2169,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2507,24 +2510,24 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J127" sqref="J127"/>
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="67.5703125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="21" customWidth="1"/>
-    <col min="9" max="10" width="25.5703125" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="17"/>
+    <col min="1" max="1" width="28.7265625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="67.54296875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="57.1796875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="21" customWidth="1"/>
+    <col min="9" max="10" width="25.54296875" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" ht="16.5">
+    <row r="1" spans="1:11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2560,7 @@
       </c>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" hidden="1">
+    <row r="2" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" hidden="1">
+    <row r="3" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5" hidden="1">
+    <row r="4" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" hidden="1">
+    <row r="5" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.5" hidden="1">
+    <row r="6" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2709,7 +2712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" hidden="1">
+    <row r="7" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" hidden="1">
+    <row r="8" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" hidden="1">
+    <row r="9" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" hidden="1">
+    <row r="10" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -2833,7 +2836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16.5" hidden="1">
+    <row r="11" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>59</v>
       </c>
@@ -2865,7 +2868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" hidden="1">
+    <row r="12" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.5" hidden="1">
+    <row r="13" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
@@ -2929,7 +2932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" hidden="1">
+    <row r="14" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>74</v>
       </c>
@@ -2961,7 +2964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5" hidden="1">
+    <row r="15" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>80</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16.5" hidden="1">
+    <row r="16" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>84</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="16.5" hidden="1">
+    <row r="17" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>90</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16.5" hidden="1">
+    <row r="18" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>95</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.5" hidden="1">
+    <row r="19" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>100</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16.5" hidden="1">
+    <row r="20" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>106</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16.5" hidden="1">
+    <row r="21" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>112</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16.5" hidden="1">
+    <row r="22" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>117</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16.5" hidden="1">
+    <row r="23" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>123</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16.5" hidden="1">
+    <row r="24" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>128</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="16.5" hidden="1">
+    <row r="25" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>133</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16.5" hidden="1">
+    <row r="26" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>140</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>80.06</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="16.5" hidden="1">
+    <row r="27" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>146</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="16.5" hidden="1">
+    <row r="28" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>151</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="16.5" hidden="1">
+    <row r="29" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>156</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="16.5" hidden="1">
+    <row r="30" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>161</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16.5" hidden="1">
+    <row r="31" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>166</v>
       </c>
@@ -3501,7 +3504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16.5" hidden="1">
+    <row r="32" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>171</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="16.5" hidden="1">
+    <row r="33" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>176</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="16.5" hidden="1">
+    <row r="34" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
         <v>182</v>
       </c>
@@ -3593,7 +3596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="16.5" hidden="1">
+    <row r="35" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>186</v>
       </c>
@@ -3625,7 +3628,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16.5" hidden="1">
+    <row r="36" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>191</v>
       </c>
@@ -3657,7 +3660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="16.5" hidden="1">
+    <row r="37" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
         <v>197</v>
       </c>
@@ -3689,7 +3692,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="16.5" hidden="1">
+    <row r="38" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
         <v>201</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="16.5" hidden="1">
+    <row r="39" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>206</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="16.5" hidden="1">
+    <row r="40" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
         <v>212</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16.5" hidden="1">
+    <row r="41" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>216</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="16.5" hidden="1">
+    <row r="42" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
         <v>222</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="16.5" hidden="1">
+    <row r="43" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>227</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="16.5" hidden="1">
+    <row r="44" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
         <v>232</v>
       </c>
@@ -3909,7 +3912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="16.5" hidden="1">
+    <row r="45" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>237</v>
       </c>
@@ -3941,7 +3944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="16.5" hidden="1">
+    <row r="46" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>242</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="16.5" hidden="1">
+    <row r="47" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>248</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="16.5" hidden="1">
+    <row r="48" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>253</v>
       </c>
@@ -4025,7 +4028,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10" ht="16.5" hidden="1">
+    <row r="49" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>256</v>
       </c>
@@ -4045,7 +4048,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10" ht="16.5" hidden="1">
+    <row r="50" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>258</v>
       </c>
@@ -4065,7 +4068,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="16.5" hidden="1">
+    <row r="51" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>260</v>
       </c>
@@ -4085,7 +4088,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10" ht="16.5" hidden="1">
+    <row r="52" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>262</v>
       </c>
@@ -4105,7 +4108,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10" ht="16.5" hidden="1">
+    <row r="53" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>264</v>
       </c>
@@ -4125,7 +4128,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" ht="16.5" hidden="1">
+    <row r="54" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>266</v>
       </c>
@@ -4145,7 +4148,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10" ht="16.5" hidden="1">
+    <row r="55" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>268</v>
       </c>
@@ -4173,7 +4176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="16.5" hidden="1">
+    <row r="56" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>273</v>
       </c>
@@ -4193,7 +4196,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="1:10" ht="16.5" hidden="1">
+    <row r="57" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>275</v>
       </c>
@@ -4213,7 +4216,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10" ht="16.5" hidden="1">
+    <row r="58" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>277</v>
       </c>
@@ -4233,7 +4236,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10" ht="16.5" hidden="1">
+    <row r="59" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>279</v>
       </c>
@@ -4253,7 +4256,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
     </row>
-    <row r="60" spans="1:10" ht="16.5" hidden="1">
+    <row r="60" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>281</v>
       </c>
@@ -4273,7 +4276,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
     </row>
-    <row r="61" spans="1:10" ht="16.5" hidden="1">
+    <row r="61" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>283</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="16.5" hidden="1">
+    <row r="62" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>287</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="16.5" hidden="1">
+    <row r="63" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>293</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="16.5" hidden="1">
+    <row r="64" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>298</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="16.5" hidden="1">
+    <row r="65" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
         <v>303</v>
       </c>
@@ -4417,7 +4420,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
     </row>
-    <row r="66" spans="1:10" ht="16.5" hidden="1">
+    <row r="66" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>305</v>
       </c>
@@ -4437,7 +4440,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
     </row>
-    <row r="67" spans="1:10" ht="16.5" hidden="1">
+    <row r="67" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>307</v>
       </c>
@@ -4457,7 +4460,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
     </row>
-    <row r="68" spans="1:10" ht="16.5" hidden="1">
+    <row r="68" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>309</v>
       </c>
@@ -4485,7 +4488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="16.5" hidden="1">
+    <row r="69" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>312</v>
       </c>
@@ -4517,7 +4520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="16.5" hidden="1">
+    <row r="70" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>317</v>
       </c>
@@ -4545,7 +4548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="16.5" hidden="1">
+    <row r="71" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>321</v>
       </c>
@@ -4565,7 +4568,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="8"/>
     </row>
-    <row r="72" spans="1:10" ht="16.5" hidden="1">
+    <row r="72" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>323</v>
       </c>
@@ -4593,7 +4596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="16.5" hidden="1">
+    <row r="73" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>327</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="16.5" hidden="1">
+    <row r="74" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>331</v>
       </c>
@@ -4653,7 +4656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="16.5" hidden="1">
+    <row r="75" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>337</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="16.5" hidden="1">
+    <row r="76" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>342</v>
       </c>
@@ -4705,7 +4708,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
     </row>
-    <row r="77" spans="1:10" ht="16.5" hidden="1">
+    <row r="77" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>344</v>
       </c>
@@ -4725,7 +4728,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="8"/>
     </row>
-    <row r="78" spans="1:10" ht="16.5" hidden="1">
+    <row r="78" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>346</v>
       </c>
@@ -4745,7 +4748,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
     </row>
-    <row r="79" spans="1:10" ht="16.5" hidden="1">
+    <row r="79" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>348</v>
       </c>
@@ -4765,7 +4768,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="8"/>
     </row>
-    <row r="80" spans="1:10" ht="16.5" hidden="1">
+    <row r="80" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>350</v>
       </c>
@@ -4785,7 +4788,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
     </row>
-    <row r="81" spans="1:10" ht="16.5" hidden="1">
+    <row r="81" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>352</v>
       </c>
@@ -4817,7 +4820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="16.5" hidden="1">
+    <row r="82" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>357</v>
       </c>
@@ -4849,7 +4852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="16.5" hidden="1">
+    <row r="83" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>361</v>
       </c>
@@ -4869,7 +4872,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
     </row>
-    <row r="84" spans="1:10" ht="16.5" hidden="1">
+    <row r="84" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
         <v>363</v>
       </c>
@@ -4889,7 +4892,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
     </row>
-    <row r="85" spans="1:10" ht="16.5" hidden="1">
+    <row r="85" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>365</v>
       </c>
@@ -4917,7 +4920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="16.5" hidden="1">
+    <row r="86" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>368</v>
       </c>
@@ -4937,7 +4940,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
     </row>
-    <row r="87" spans="1:10" ht="16.5" hidden="1">
+    <row r="87" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>370</v>
       </c>
@@ -4969,7 +4972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="16.5" hidden="1">
+    <row r="88" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
         <v>375</v>
       </c>
@@ -4989,7 +4992,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
     </row>
-    <row r="89" spans="1:10" ht="16.5" hidden="1">
+    <row r="89" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>377</v>
       </c>
@@ -5017,7 +5020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="16.5" hidden="1">
+    <row r="90" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
         <v>381</v>
       </c>
@@ -5037,7 +5040,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
     </row>
-    <row r="91" spans="1:10" ht="16.5" hidden="1">
+    <row r="91" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
         <v>383</v>
       </c>
@@ -5057,7 +5060,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="8"/>
     </row>
-    <row r="92" spans="1:10" ht="16.5" hidden="1">
+    <row r="92" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
         <v>385</v>
       </c>
@@ -5077,7 +5080,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
     </row>
-    <row r="93" spans="1:10" ht="16.5" hidden="1">
+    <row r="93" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
         <v>387</v>
       </c>
@@ -5097,7 +5100,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="8"/>
     </row>
-    <row r="94" spans="1:10" ht="16.5" hidden="1">
+    <row r="94" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
         <v>389</v>
       </c>
@@ -5117,7 +5120,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
     </row>
-    <row r="95" spans="1:10" ht="16.5" hidden="1">
+    <row r="95" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>391</v>
       </c>
@@ -5137,7 +5140,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="8"/>
     </row>
-    <row r="96" spans="1:10" ht="16.5" hidden="1">
+    <row r="96" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>393</v>
       </c>
@@ -5165,7 +5168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="16.5" hidden="1">
+    <row r="97" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
         <v>397</v>
       </c>
@@ -5185,7 +5188,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="8"/>
     </row>
-    <row r="98" spans="1:10" ht="16.5" hidden="1">
+    <row r="98" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>399</v>
       </c>
@@ -5217,7 +5220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="16.5" hidden="1">
+    <row r="99" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
         <v>404</v>
       </c>
@@ -5237,7 +5240,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="8"/>
     </row>
-    <row r="100" spans="1:10" ht="16.5" hidden="1">
+    <row r="100" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="6" t="s">
         <v>406</v>
       </c>
@@ -5257,7 +5260,7 @@
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
     </row>
-    <row r="101" spans="1:10" ht="16.5" hidden="1">
+    <row r="101" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
         <v>408</v>
       </c>
@@ -5277,7 +5280,7 @@
       <c r="I101" s="8"/>
       <c r="J101" s="8"/>
     </row>
-    <row r="102" spans="1:10" ht="15" hidden="1">
+    <row r="102" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>410</v>
       </c>
@@ -5301,7 +5304,7 @@
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
     </row>
-    <row r="103" spans="1:10" ht="16.5" hidden="1">
+    <row r="103" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>416</v>
       </c>
@@ -5333,7 +5336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="16.5" hidden="1">
+    <row r="104" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>422</v>
       </c>
@@ -5365,7 +5368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="16.5" hidden="1">
+    <row r="105" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>426</v>
       </c>
@@ -5391,7 +5394,7 @@
       <c r="I105" s="8"/>
       <c r="J105" s="8"/>
     </row>
-    <row r="106" spans="1:10" ht="16.5" hidden="1">
+    <row r="106" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>430</v>
       </c>
@@ -5423,7 +5426,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" hidden="1">
+    <row r="107" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>434</v>
       </c>
@@ -5451,7 +5454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15" hidden="1">
+    <row r="108" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>438</v>
       </c>
@@ -5479,7 +5482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="16.5" hidden="1">
+    <row r="109" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>441</v>
       </c>
@@ -5511,7 +5514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="16.5" hidden="1">
+    <row r="110" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>445</v>
       </c>
@@ -5543,7 +5546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="16.5" hidden="1">
+    <row r="111" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>449</v>
       </c>
@@ -5575,7 +5578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="16.5" hidden="1">
+    <row r="112" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>453</v>
       </c>
@@ -5607,7 +5610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="16.5" hidden="1">
+    <row r="113" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>457</v>
       </c>
@@ -5634,7 +5637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="16.5" hidden="1">
+    <row r="114" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>461</v>
       </c>
@@ -5662,7 +5665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="16.5" hidden="1">
+    <row r="115" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>464</v>
       </c>
@@ -5690,7 +5693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="16.5" hidden="1">
+    <row r="116" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>468</v>
       </c>
@@ -5718,7 +5721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="16.5" hidden="1">
+    <row r="117" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>472</v>
       </c>
@@ -5746,7 +5749,7 @@
       <c r="I117" s="8"/>
       <c r="J117" s="8"/>
     </row>
-    <row r="118" spans="1:10" ht="16.5" hidden="1">
+    <row r="118" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>478</v>
       </c>
@@ -5774,7 +5777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="16.5" hidden="1">
+    <row r="119" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>482</v>
       </c>
@@ -5806,7 +5809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="16.5" hidden="1">
+    <row r="120" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>489</v>
       </c>
@@ -5832,7 +5835,7 @@
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
     </row>
-    <row r="121" spans="1:10" ht="16.5" hidden="1">
+    <row r="121" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>494</v>
       </c>
@@ -5860,7 +5863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="16.5" hidden="1">
+    <row r="122" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>499</v>
       </c>
@@ -5888,7 +5891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="16.5" hidden="1">
+    <row r="123" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>504</v>
       </c>
@@ -5912,7 +5915,7 @@
       <c r="I123" s="8"/>
       <c r="J123" s="8"/>
     </row>
-    <row r="124" spans="1:10" ht="16.5" hidden="1">
+    <row r="124" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>509</v>
       </c>
@@ -5936,7 +5939,7 @@
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
     </row>
-    <row r="125" spans="1:10" ht="18" hidden="1" customHeight="1">
+    <row r="125" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>514</v>
       </c>
@@ -5960,7 +5963,7 @@
       <c r="I125" s="8"/>
       <c r="J125" s="8"/>
     </row>
-    <row r="126" spans="1:10" ht="16.5" hidden="1">
+    <row r="126" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>519</v>
       </c>
@@ -5984,7 +5987,7 @@
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>
     </row>
-    <row r="127" spans="1:10" s="35" customFormat="1" ht="16.5">
+    <row r="127" spans="1:10" s="35" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A127" s="30" t="s">
         <v>523</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="35" customFormat="1" ht="16.5">
+    <row r="128" spans="1:10" s="35" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A128" s="30" t="s">
         <v>532</v>
       </c>
@@ -6040,7 +6043,7 @@
       <c r="I128" s="36"/>
       <c r="J128" s="36"/>
     </row>
-    <row r="129" spans="1:10" ht="33">
+    <row r="129" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>536</v>
       </c>
@@ -6070,7 +6073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="33">
+    <row r="130" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>541</v>
       </c>
@@ -6100,7 +6103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="33">
+    <row r="131" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>545</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="16.5">
+    <row r="132" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>549</v>
       </c>
@@ -6160,7 +6163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="33">
+    <row r="133" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>554</v>
       </c>
@@ -6190,7 +6193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="16.5">
+    <row r="134" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>558</v>
       </c>
@@ -6220,7 +6223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="16.5">
+    <row r="135" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>562</v>
       </c>
@@ -6250,7 +6253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="16.5">
+    <row r="136" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>566</v>
       </c>
@@ -6280,7 +6283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="16.5">
+    <row r="137" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>570</v>
       </c>
@@ -6310,7 +6313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="16.5">
+    <row r="138" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>574</v>
       </c>
@@ -6340,7 +6343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="16.5">
+    <row r="139" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>577</v>
       </c>
@@ -6370,7 +6373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="16.5">
+    <row r="140" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>581</v>
       </c>
@@ -6400,15 +6403,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="33">
+    <row r="141" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>584</v>
       </c>
       <c r="B141" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="C141" s="16" t="s">
         <v>585</v>
-      </c>
-      <c r="C141" s="16" t="s">
-        <v>586</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>13</v>
@@ -6421,7 +6424,7 @@
       </c>
       <c r="G141" s="8"/>
       <c r="H141" s="14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I141" s="8" t="s">
         <v>531</v>
@@ -6430,15 +6433,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="16.5">
+    <row r="142" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B142" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="C142" s="16" t="s">
         <v>589</v>
-      </c>
-      <c r="C142" s="16" t="s">
-        <v>590</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>13</v>
@@ -6447,26 +6450,26 @@
         <v>527</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G142" s="8"/>
       <c r="H142" s="14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I142" s="8"/>
       <c r="J142" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="16.5">
+    <row r="143" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B143" s="4" t="s">
-        <v>594</v>
-      </c>
       <c r="C143" s="16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>13</v>
@@ -6475,26 +6478,26 @@
         <v>527</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G143" s="8"/>
       <c r="H143" s="14" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I143" s="8"/>
       <c r="J143" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="16.5">
+    <row r="144" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="B144" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="B144" s="4" t="s">
-        <v>597</v>
-      </c>
       <c r="C144" s="16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>13</v>
@@ -6503,155 +6506,155 @@
         <v>527</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G144" s="8"/>
       <c r="H144" s="14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I144" s="8"/>
       <c r="J144" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="15" hidden="1">
+    <row r="145" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A145" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B145" s="37" t="s">
         <v>599</v>
       </c>
-      <c r="B145" s="37" t="s">
+      <c r="C145" s="37" t="s">
         <v>600</v>
       </c>
-      <c r="C145" s="37" t="s">
+      <c r="D145" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="D145" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E145" s="3" t="s">
+      <c r="F145" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="F145" s="8" t="s">
-        <v>603</v>
       </c>
       <c r="G145" s="8"/>
       <c r="H145" s="14"/>
       <c r="I145" s="8"/>
       <c r="J145" s="8"/>
     </row>
-    <row r="146" spans="1:10" ht="15" hidden="1">
+    <row r="146" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A146" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="B146" s="37" t="s">
         <v>604</v>
       </c>
-      <c r="B146" s="37" t="s">
+      <c r="C146" s="37" t="s">
         <v>605</v>
       </c>
-      <c r="C146" s="37" t="s">
+      <c r="D146" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F146" s="5" t="s">
         <v>606</v>
-      </c>
-      <c r="D146" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="F146" s="5" t="s">
-        <v>607</v>
       </c>
       <c r="G146" s="8"/>
       <c r="H146" s="14"/>
       <c r="I146" s="8"/>
       <c r="J146" s="8"/>
     </row>
-    <row r="147" spans="1:10" ht="15" hidden="1">
+    <row r="147" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A147" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="B147" s="37" t="s">
         <v>608</v>
       </c>
-      <c r="B147" s="37" t="s">
+      <c r="C147" s="37" t="s">
         <v>609</v>
       </c>
-      <c r="C147" s="37" t="s">
+      <c r="D147" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F147" s="9" t="s">
         <v>610</v>
-      </c>
-      <c r="D147" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="F147" s="9" t="s">
-        <v>611</v>
       </c>
       <c r="G147" s="8"/>
       <c r="H147" s="14"/>
       <c r="I147" s="8"/>
       <c r="J147" s="8"/>
     </row>
-    <row r="148" spans="1:10" ht="15" hidden="1">
+    <row r="148" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A148" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="B148" s="37" t="s">
         <v>612</v>
       </c>
-      <c r="B148" s="37" t="s">
+      <c r="C148" s="37" t="s">
         <v>613</v>
       </c>
-      <c r="C148" s="37" t="s">
-        <v>614</v>
-      </c>
       <c r="D148" s="38" t="s">
         <v>13</v>
       </c>
       <c r="E148" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F148" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="F148" s="8" t="s">
-        <v>603</v>
       </c>
       <c r="G148" s="8"/>
       <c r="H148" s="14"/>
       <c r="I148" s="8"/>
       <c r="J148" s="8"/>
     </row>
-    <row r="149" spans="1:10" ht="15" hidden="1">
+    <row r="149" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A149" s="29" t="s">
+        <v>614</v>
+      </c>
+      <c r="B149" s="37" t="s">
         <v>615</v>
       </c>
-      <c r="B149" s="37" t="s">
+      <c r="C149" s="37" t="s">
         <v>616</v>
       </c>
-      <c r="C149" s="37" t="s">
+      <c r="D149" s="38" t="s">
         <v>617</v>
       </c>
-      <c r="D149" s="38" t="s">
+      <c r="E149" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F149" s="29" t="s">
         <v>618</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="F149" s="29" t="s">
-        <v>619</v>
       </c>
       <c r="G149" s="28"/>
       <c r="H149" s="28"/>
       <c r="I149" s="28"/>
       <c r="J149" s="28"/>
     </row>
-    <row r="150" spans="1:10" ht="15" hidden="1">
+    <row r="150" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="A150" s="29" t="s">
+        <v>619</v>
+      </c>
+      <c r="B150" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="B150" s="37" t="s">
+      <c r="C150" s="37" t="s">
         <v>621</v>
       </c>
-      <c r="C150" s="37" t="s">
+      <c r="D150" s="38" t="s">
         <v>622</v>
       </c>
-      <c r="D150" s="38" t="s">
-        <v>623</v>
-      </c>
       <c r="E150" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F150" s="29" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G150" s="28"/>
       <c r="H150" s="28"/>
@@ -6665,22 +6668,17 @@
         <filter val="PT"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A127:K144">
+      <sortCondition ref="A1:A150"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8">
@@ -6690,6 +6688,15 @@
     <Comment xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6908,13 +6915,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD8E79D5-88FA-489E-8500-1B15CD65140C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A9289C4-D150-42AA-B6FF-66D9C6607C50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
+    <ds:schemaRef ds:uri="9f04ef3f-090d-46e3-96be-1fbea4829461"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A9289C4-D150-42AA-B6FF-66D9C6607C50}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD8E79D5-88FA-489E-8500-1B15CD65140C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3EC13CA-7BDB-4D66-8673-9D7BF7DB0AE6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3EC13CA-7BDB-4D66-8673-9D7BF7DB0AE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
+    <ds:schemaRef ds:uri="9f04ef3f-090d-46e3-96be-1fbea4829461"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>